<commit_message>
Changed a value in the Data excel
</commit_message>
<xml_diff>
--- a/Data/Dollars.xlsx
+++ b/Data/Dollars.xlsx
@@ -48,7 +48,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -71,13 +71,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -360,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,6 +410,11 @@
         <v>45</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>